<commit_message>
Separated Mods into own CFG
</commit_message>
<xml_diff>
--- a/Historical Progression Tech Tree.xlsx
+++ b/Historical Progression Tech Tree.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pap\Dropbox\KSP\Git\HPTechTree\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="27795" windowHeight="12090"/>
+    <workbookView xWindow="480" yWindow="390" windowWidth="27795" windowHeight="12030"/>
   </bookViews>
   <sheets>
     <sheet name="Tech Tree" sheetId="1" r:id="rId1"/>
@@ -17,12 +12,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Tech Tree'!$A$1:$W$113</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="610">
   <si>
     <t>1957-1958</t>
   </si>
@@ -145,9 +140,6 @@
   </si>
   <si>
     <t>LEVEL 13</t>
-  </si>
-  <si>
-    <t>15-18-20</t>
   </si>
   <si>
     <t>START</t>
@@ -2051,7 +2043,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2086,7 +2078,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2297,9 +2289,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="25" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A105" sqref="A105"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" zoomScaleSheetLayoutView="25" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2358,13 +2350,13 @@
         <v>3</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>536</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>537</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>4</v>
@@ -2454,17 +2446,17 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="I4" s="11" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="O4" s="11"/>
       <c r="Q4" s="11" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="U4" s="11" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -2508,13 +2500,13 @@
         <v>40</v>
       </c>
       <c r="AA5" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="AC5" s="1" t="s">
         <v>542</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AE5" s="1" t="s">
         <v>543</v>
-      </c>
-      <c r="AE5" s="1" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -2524,44 +2516,89 @@
       <c r="C6" s="1">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>41</v>
+      <c r="D6" s="1">
+        <f>C6/5</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1">
+        <v>5</v>
       </c>
       <c r="G6" s="1">
         <v>45</v>
       </c>
+      <c r="H6" s="1">
+        <f>G6/E6</f>
+        <v>3</v>
+      </c>
       <c r="I6" s="1">
         <v>90</v>
       </c>
+      <c r="J6" s="1">
+        <f>I6/G6</f>
+        <v>2</v>
+      </c>
       <c r="K6" s="1">
         <v>160</v>
       </c>
+      <c r="L6" s="1">
+        <v>160</v>
+      </c>
       <c r="M6" s="1">
         <v>300</v>
       </c>
+      <c r="N6" s="1">
+        <v>300</v>
+      </c>
       <c r="O6" s="1">
         <v>550</v>
       </c>
+      <c r="P6" s="1">
+        <v>500</v>
+      </c>
       <c r="Q6" s="1">
         <v>1000</v>
       </c>
+      <c r="R6" s="1">
+        <v>700</v>
+      </c>
       <c r="S6" s="1">
         <v>1500</v>
       </c>
+      <c r="T6" s="1">
+        <v>900</v>
+      </c>
       <c r="U6" s="1">
         <v>2250</v>
       </c>
+      <c r="V6" s="1">
+        <v>1100</v>
+      </c>
       <c r="W6" s="1">
         <v>4000</v>
       </c>
+      <c r="X6" s="1">
+        <v>1300</v>
+      </c>
       <c r="Y6" s="1">
         <v>4000</v>
       </c>
+      <c r="Z6" s="1">
+        <v>1500</v>
+      </c>
       <c r="AA6" s="1">
         <v>4000</v>
       </c>
+      <c r="AB6" s="1">
+        <v>1700</v>
+      </c>
       <c r="AC6" s="1">
         <v>4000</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>1900</v>
       </c>
       <c r="AE6" s="1">
         <v>10000</v>
@@ -2616,141 +2653,141 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1">
         <v>1665</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="S8" s="12" t="s">
+        <v>533</v>
+      </c>
+      <c r="U8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="S8" s="12" t="s">
-        <v>534</v>
-      </c>
-      <c r="U8" s="2" t="s">
+      <c r="W8" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="Y8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="W8" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AA8" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="AC8" s="2" t="s">
         <v>563</v>
-      </c>
-      <c r="AC8" s="2" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="K9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="Q9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="Q9" s="3" t="s">
+      <c r="S9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="S9" s="3" t="s">
+      <c r="U9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="U9" s="3" t="s">
-        <v>63</v>
-      </c>
       <c r="W9" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L10" s="5"/>
       <c r="M10" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P10" s="5"/>
       <c r="Q10" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R10" s="5"/>
       <c r="S10" s="4"/>
       <c r="T10" s="5"/>
       <c r="U10" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V10" s="5"/>
       <c r="W10" s="4"/>
@@ -2760,38 +2797,38 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N11" s="5"/>
       <c r="O11" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P11" s="5"/>
       <c r="Q11" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R11" s="5"/>
       <c r="S11" s="4"/>
@@ -2812,15 +2849,15 @@
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
       <c r="I12" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="N12" s="5"/>
       <c r="O12" s="4"/>
@@ -2847,7 +2884,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="5"/>
       <c r="K13" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13" s="4"/>
@@ -3020,121 +3057,121 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B19" s="1">
         <v>1545</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="K19" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="O19" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="O19" s="2" t="s">
+      <c r="Q19" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="S19" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="S19" s="2" t="s">
+      <c r="U19" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="U19" s="2" t="s">
+      <c r="W19" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="Y19" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="W19" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="Y19" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="AA19" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="AC19" s="2" t="s">
         <v>566</v>
-      </c>
-      <c r="AC19" s="2" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="C20" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="K20" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="M20" s="3" t="s">
+      <c r="O20" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="O20" s="3" t="s">
+      <c r="Q20" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="Q20" s="3" t="s">
+      <c r="S20" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="S20" s="3" t="s">
+      <c r="U20" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="U20" s="3" t="s">
+      <c r="W20" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="Y20" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="W20" s="3" t="s">
-        <v>561</v>
-      </c>
-      <c r="Y20" s="3" t="s">
-        <v>108</v>
-      </c>
       <c r="AA20" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="AC20" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="4"/>
       <c r="F21" s="5"/>
       <c r="G21" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="6"/>
       <c r="J21" s="5"/>
       <c r="K21" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L21" s="5"/>
       <c r="M21" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N21" s="5"/>
       <c r="O21" s="6"/>
@@ -3144,7 +3181,7 @@
       <c r="S21" s="4"/>
       <c r="T21" s="5"/>
       <c r="U21" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V21" s="5"/>
       <c r="W21" s="4"/>
@@ -3389,137 +3426,137 @@
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B30" s="1">
         <v>1425</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="K30" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="M30" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="M30" s="2" t="s">
+      <c r="O30" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="O30" s="2" t="s">
+      <c r="Q30" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="Q30" s="2" t="s">
+      <c r="S30" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="S30" s="2" t="s">
+      <c r="U30" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="U30" s="2" t="s">
+      <c r="W30" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="Y30" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="W30" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="Y30" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="AA30" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="AC30" s="2" t="s">
         <v>569</v>
-      </c>
-      <c r="AC30" s="2" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="C31" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="I31" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="K31" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="M31" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="M31" s="3" t="s">
+      <c r="O31" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="O31" s="3" t="s">
+      <c r="Q31" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="Q31" s="3" t="s">
+      <c r="S31" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="S31" s="3" t="s">
+      <c r="U31" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="U31" s="3" t="s">
+      <c r="W31" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="Y31" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="W31" s="3" t="s">
-        <v>560</v>
-      </c>
-      <c r="Y31" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="AA31" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="AC31" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>138</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J32" s="5"/>
       <c r="K32" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L32" s="5"/>
       <c r="M32" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N32" s="5"/>
       <c r="O32" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P32" s="5"/>
       <c r="Q32" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="R32" s="5"/>
       <c r="S32" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="T32" s="5"/>
       <c r="U32" s="7"/>
@@ -3531,38 +3568,38 @@
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>147</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J33" s="5"/>
       <c r="K33" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L33" s="5"/>
       <c r="M33" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N33" s="5"/>
       <c r="O33" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P33" s="5"/>
       <c r="Q33" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="R33" s="5"/>
       <c r="S33" s="4"/>
@@ -3576,32 +3613,32 @@
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="4"/>
       <c r="H34" s="5"/>
       <c r="I34" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L34" s="5"/>
       <c r="M34" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="N34" s="5"/>
       <c r="O34" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P34" s="5"/>
       <c r="Q34" s="4"/>
@@ -3617,10 +3654,10 @@
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="4"/>
@@ -3628,19 +3665,19 @@
       <c r="G35" s="4"/>
       <c r="H35" s="5"/>
       <c r="I35" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J35" s="5"/>
       <c r="K35" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L35" s="5"/>
       <c r="M35" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="N35" s="5"/>
       <c r="O35" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P35" s="5"/>
       <c r="Q35" s="4"/>
@@ -3663,19 +3700,19 @@
       <c r="G36" s="4"/>
       <c r="H36" s="5"/>
       <c r="I36" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J36" s="5"/>
       <c r="K36" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L36" s="5"/>
       <c r="M36" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N36" s="5"/>
       <c r="O36" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P36" s="5"/>
       <c r="Q36" s="4"/>
@@ -3702,11 +3739,11 @@
       <c r="K37" s="4"/>
       <c r="L37" s="5"/>
       <c r="M37" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N37" s="5"/>
       <c r="O37" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P37" s="5"/>
       <c r="Q37" s="4"/>
@@ -3735,7 +3772,7 @@
       <c r="M38" s="4"/>
       <c r="N38" s="5"/>
       <c r="O38" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P38" s="5"/>
       <c r="Q38" s="4"/>
@@ -3764,7 +3801,7 @@
       <c r="M39" s="4"/>
       <c r="N39" s="5"/>
       <c r="O39" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P39" s="5"/>
       <c r="Q39" s="4"/>
@@ -3787,7 +3824,7 @@
       <c r="K40" s="8"/>
       <c r="M40" s="8"/>
       <c r="O40" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q40" s="8"/>
       <c r="S40" s="8"/>
@@ -3844,108 +3881,108 @@
     </row>
     <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B42" s="1">
         <v>1305</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="I42" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="I42" s="2" t="s">
+      <c r="K42" s="12" t="s">
+        <v>526</v>
+      </c>
+      <c r="M42" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="K42" s="12" t="s">
-        <v>527</v>
-      </c>
-      <c r="M42" s="2" t="s">
+      <c r="O42" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="O42" s="12" t="s">
+      <c r="Q42" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="S42" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="U42" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="Q42" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="S42" s="2" t="s">
+      <c r="W42" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="Y42" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="U42" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="W42" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="Y42" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="AA42" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="AC42" s="2" t="s">
         <v>572</v>
-      </c>
-      <c r="AC42" s="2" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="C43" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D43" s="11"/>
       <c r="E43" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H43" s="11"/>
       <c r="I43" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J43" s="11"/>
       <c r="K43" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L43" s="11"/>
       <c r="M43" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N43" s="11"/>
       <c r="O43" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P43" s="11"/>
       <c r="Q43" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="R43" s="11"/>
       <c r="S43" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T43" s="11"/>
       <c r="U43" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="V43" s="11"/>
       <c r="W43" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="X43" s="11"/>
       <c r="Y43" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AA43" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="AC43" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="AD43" s="11"/>
       <c r="AE43" s="11"/>
@@ -3953,34 +3990,34 @@
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>199</v>
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F44" s="5"/>
       <c r="G44" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J44" s="5"/>
       <c r="K44" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L44" s="5"/>
       <c r="M44" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N44" s="5"/>
       <c r="O44" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P44" s="5"/>
       <c r="Q44" s="6"/>
@@ -3996,32 +4033,32 @@
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>207</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="6"/>
       <c r="L45" s="5"/>
       <c r="M45" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N45" s="5"/>
       <c r="O45" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="P45" s="5"/>
       <c r="Q45" s="4"/>
@@ -4037,28 +4074,28 @@
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="5"/>
       <c r="E46" s="4"/>
       <c r="F46" s="5"/>
       <c r="G46" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J46" s="5"/>
       <c r="K46" s="7"/>
       <c r="L46" s="5"/>
       <c r="M46" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N46" s="5"/>
       <c r="O46" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="P46" s="5"/>
       <c r="Q46" s="4"/>
@@ -4074,14 +4111,14 @@
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="5"/>
       <c r="E47" s="4"/>
       <c r="F47" s="5"/>
       <c r="G47" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="4"/>
@@ -4089,11 +4126,11 @@
       <c r="K47" s="4"/>
       <c r="L47" s="5"/>
       <c r="M47" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N47" s="5"/>
       <c r="O47" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="P47" s="5"/>
       <c r="Q47" s="4"/>
@@ -4109,7 +4146,7 @@
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="5"/>
@@ -4122,11 +4159,11 @@
       <c r="K48" s="4"/>
       <c r="L48" s="5"/>
       <c r="M48" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N48" s="5"/>
       <c r="O48" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P48" s="5"/>
       <c r="Q48" s="4"/>
@@ -4142,7 +4179,7 @@
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="5"/>
@@ -4290,158 +4327,158 @@
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B54" s="1">
         <v>1185</v>
       </c>
       <c r="C54" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="I54" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="I54" s="2" t="s">
+      <c r="K54" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="K54" s="2" t="s">
+      <c r="M54" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="M54" s="2" t="s">
+      <c r="O54" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="O54" s="2" t="s">
+      <c r="Q54" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="Q54" s="2" t="s">
+      <c r="S54" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="S54" s="2" t="s">
+      <c r="U54" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="U54" s="2" t="s">
+      <c r="W54" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="Y54" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="W54" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="Y54" s="2" t="s">
-        <v>236</v>
-      </c>
       <c r="AA54" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="AC54" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="AC54" s="2" t="s">
-        <v>576</v>
-      </c>
       <c r="AE54" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="C55" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D55" s="11"/>
       <c r="E55" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F55" s="11"/>
       <c r="G55" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H55" s="11"/>
       <c r="I55" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J55" s="11"/>
       <c r="K55" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L55" s="11"/>
       <c r="M55" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N55" s="11"/>
       <c r="O55" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P55" s="11"/>
       <c r="Q55" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="R55" s="11"/>
       <c r="S55" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="T55" s="11"/>
       <c r="U55" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="V55" s="11"/>
       <c r="W55" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="X55" s="11"/>
       <c r="Y55" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AA55" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="AC55" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="AE55" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="D56" s="5"/>
       <c r="E56" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F56" s="5"/>
       <c r="G56" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H56" s="5"/>
       <c r="I56" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J56" s="5"/>
       <c r="K56" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L56" s="5"/>
       <c r="M56" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N56" s="5"/>
       <c r="O56" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="P56" s="5"/>
       <c r="Q56" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="R56" s="5"/>
       <c r="S56" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="T56" s="5"/>
       <c r="U56" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="V56" s="5"/>
       <c r="W56" s="4"/>
@@ -4452,34 +4489,34 @@
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>258</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>259</v>
       </c>
       <c r="D57" s="5"/>
       <c r="E57" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F57" s="5"/>
       <c r="G57" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J57" s="5"/>
       <c r="K57" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="L57" s="5"/>
       <c r="M57" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N57" s="5"/>
       <c r="O57" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P57" s="5"/>
       <c r="Q57" s="4"/>
@@ -4487,7 +4524,7 @@
       <c r="S57" s="4"/>
       <c r="T57" s="5"/>
       <c r="U57" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="V57" s="5"/>
       <c r="W57" s="4"/>
@@ -4498,34 +4535,34 @@
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>268</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>269</v>
       </c>
       <c r="D58" s="5"/>
       <c r="E58" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F58" s="5"/>
       <c r="G58" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H58" s="5"/>
       <c r="I58" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J58" s="5"/>
       <c r="K58" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L58" s="5"/>
       <c r="M58" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="N58" s="5"/>
       <c r="O58" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P58" s="5"/>
       <c r="Q58" s="6"/>
@@ -4542,34 +4579,34 @@
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>278</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>279</v>
       </c>
       <c r="D59" s="5"/>
       <c r="E59" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F59" s="5"/>
       <c r="G59" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J59" s="5"/>
       <c r="K59" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L59" s="5"/>
       <c r="M59" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="N59" s="5"/>
       <c r="O59" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P59" s="5"/>
       <c r="Q59" s="4"/>
@@ -4586,34 +4623,34 @@
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>286</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>287</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F60" s="5"/>
       <c r="G60" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H60" s="5"/>
       <c r="I60" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J60" s="5"/>
       <c r="K60" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L60" s="5"/>
       <c r="M60" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="N60" s="5"/>
       <c r="O60" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P60" s="5"/>
       <c r="Q60" s="4"/>
@@ -4630,30 +4667,30 @@
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>294</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>295</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F61" s="5"/>
       <c r="G61" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J61" s="5"/>
       <c r="K61" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L61" s="5"/>
       <c r="M61" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N61" s="5"/>
       <c r="O61" s="6"/>
@@ -4672,32 +4709,32 @@
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>302</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>303</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="4"/>
       <c r="F62" s="5"/>
       <c r="G62" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J62" s="5"/>
       <c r="K62" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L62" s="5"/>
       <c r="M62" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="N62" s="5"/>
       <c r="O62" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P62" s="5"/>
       <c r="Q62" s="4"/>
@@ -4714,26 +4751,26 @@
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="5"/>
       <c r="E63" s="4"/>
       <c r="F63" s="5"/>
       <c r="G63" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J63" s="5"/>
       <c r="K63" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L63" s="5"/>
       <c r="M63" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N63" s="5"/>
       <c r="O63" s="4"/>
@@ -4763,7 +4800,7 @@
       <c r="K64" s="4"/>
       <c r="L64" s="5"/>
       <c r="M64" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N64" s="5"/>
       <c r="O64" s="4"/>
@@ -4786,13 +4823,13 @@
       <c r="E65" s="8"/>
       <c r="G65" s="8"/>
       <c r="I65" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K65" s="8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="M65" s="8" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="O65" s="10"/>
       <c r="Q65" s="8"/>
@@ -4851,133 +4888,133 @@
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B67" s="1">
         <v>1065</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="G67" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="I67" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="I67" s="2" t="s">
+      <c r="K67" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="K67" s="2" t="s">
+      <c r="M67" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="M67" s="2" t="s">
+      <c r="O67" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="O67" s="2" t="s">
+      <c r="Q67" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="Q67" s="2" t="s">
+      <c r="S67" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="S67" s="2" t="s">
+      <c r="U67" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="U67" s="2" t="s">
+      <c r="W67" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="Y67" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="W67" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="Y67" s="2" t="s">
-        <v>322</v>
-      </c>
       <c r="AA67" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="AC67" s="2" t="s">
         <v>578</v>
-      </c>
-      <c r="AC67" s="2" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="C68" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="G68" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="G68" s="3" t="s">
+      <c r="I68" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="I68" s="3" t="s">
+      <c r="K68" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="K68" s="3" t="s">
+      <c r="M68" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="M68" s="3" t="s">
+      <c r="O68" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="O68" s="3" t="s">
+      <c r="Q68" s="3" t="s">
         <v>329</v>
       </c>
-      <c r="Q68" s="3" t="s">
+      <c r="S68" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="S68" s="3" t="s">
+      <c r="U68" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="U68" s="3" t="s">
+      <c r="W68" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="Y68" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="W68" s="3" t="s">
-        <v>557</v>
-      </c>
-      <c r="Y68" s="3" t="s">
-        <v>333</v>
-      </c>
       <c r="AA68" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="AC68" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>334</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>335</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F69" s="5"/>
       <c r="G69" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H69" s="5"/>
       <c r="I69" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J69" s="5"/>
       <c r="K69" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="L69" s="5"/>
       <c r="M69" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="N69" s="5"/>
       <c r="O69" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="P69" s="5"/>
       <c r="Q69" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="R69" s="5"/>
       <c r="S69" s="4"/>
@@ -4992,33 +5029,33 @@
     <row r="70" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="C70" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F70" s="5"/>
       <c r="G70" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H70" s="5"/>
       <c r="I70" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J70" s="5"/>
       <c r="K70" s="6"/>
       <c r="L70" s="5"/>
       <c r="M70" s="7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N70" s="5"/>
       <c r="O70" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P70" s="5"/>
       <c r="Q70" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="R70" s="5"/>
       <c r="S70" s="4"/>
@@ -5035,27 +5072,27 @@
       <c r="C71" s="4"/>
       <c r="D71" s="5"/>
       <c r="E71" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F71" s="5"/>
       <c r="G71" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H71" s="5"/>
       <c r="I71" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J71" s="5"/>
       <c r="K71" s="7"/>
       <c r="L71" s="5"/>
       <c r="M71" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="N71" s="5"/>
       <c r="O71" s="4"/>
       <c r="P71" s="5"/>
       <c r="Q71" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="R71" s="5"/>
       <c r="S71" s="4"/>
@@ -5074,23 +5111,23 @@
       <c r="E72" s="4"/>
       <c r="F72" s="5"/>
       <c r="G72" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H72" s="5"/>
       <c r="I72" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J72" s="5"/>
       <c r="K72" s="4"/>
       <c r="L72" s="5"/>
       <c r="M72" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="N72" s="5"/>
       <c r="O72" s="4"/>
       <c r="P72" s="5"/>
       <c r="Q72" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="R72" s="5"/>
       <c r="S72" s="4"/>
@@ -5107,11 +5144,11 @@
       <c r="C73" s="4"/>
       <c r="D73" s="5"/>
       <c r="E73" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F73" s="5"/>
       <c r="G73" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H73" s="5"/>
       <c r="I73" s="4"/>
@@ -5119,7 +5156,7 @@
       <c r="K73" s="4"/>
       <c r="L73" s="5"/>
       <c r="M73" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N73" s="5"/>
       <c r="O73" s="4"/>
@@ -5142,7 +5179,7 @@
       <c r="E74" s="4"/>
       <c r="F74" s="5"/>
       <c r="G74" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H74" s="5"/>
       <c r="I74" s="4"/>
@@ -5282,129 +5319,129 @@
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B79" s="1">
         <v>945</v>
       </c>
       <c r="C79" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="I79" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="K79" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="K79" s="2" t="s">
+      <c r="M79" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="M79" s="2" t="s">
+      <c r="O79" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="O79" s="2" t="s">
+      <c r="Q79" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="Q79" s="2" t="s">
+      <c r="S79" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="S79" s="2" t="s">
+      <c r="U79" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="U79" s="2" t="s">
+      <c r="W79" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="Y79" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="W79" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="Y79" s="2" t="s">
-        <v>372</v>
-      </c>
       <c r="AA79" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AC79" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="AC79" s="2" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="C80" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="E80" s="3" t="s">
         <v>373</v>
       </c>
-      <c r="E80" s="3" t="s">
+      <c r="G80" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="G80" s="3" t="s">
+      <c r="I80" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="I80" s="3" t="s">
+      <c r="K80" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="K80" s="3" t="s">
+      <c r="M80" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="M80" s="3" t="s">
+      <c r="O80" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="O80" s="3" t="s">
+      <c r="Q80" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="Q80" s="3" t="s">
+      <c r="S80" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="S80" s="3" t="s">
+      <c r="U80" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="U80" s="3" t="s">
+      <c r="W80" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="Y80" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="W80" s="3" t="s">
-        <v>556</v>
-      </c>
-      <c r="Y80" s="3" t="s">
-        <v>383</v>
-      </c>
       <c r="AA80" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="AC80" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="81" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C81" s="4" t="s">
         <v>384</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>385</v>
       </c>
       <c r="D81" s="5"/>
       <c r="E81" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F81" s="5"/>
       <c r="G81" s="4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H81" s="5"/>
       <c r="I81" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J81" s="5"/>
       <c r="K81" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L81" s="5"/>
       <c r="M81" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="N81" s="5"/>
       <c r="O81" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="P81" s="5"/>
       <c r="Q81" s="6"/>
@@ -5423,23 +5460,23 @@
       <c r="C82" s="4"/>
       <c r="D82" s="5"/>
       <c r="E82" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F82" s="5"/>
       <c r="G82" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H82" s="5"/>
       <c r="I82" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J82" s="5"/>
       <c r="K82" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L82" s="5"/>
       <c r="M82" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N82" s="5"/>
       <c r="O82" s="4"/>
@@ -5462,19 +5499,19 @@
       <c r="E83" s="4"/>
       <c r="F83" s="5"/>
       <c r="G83" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H83" s="5"/>
       <c r="I83" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J83" s="5"/>
       <c r="K83" s="7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L83" s="5"/>
       <c r="M83" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="N83" s="5"/>
       <c r="O83" s="4"/>
@@ -5497,17 +5534,17 @@
       <c r="E84" s="4"/>
       <c r="F84" s="5"/>
       <c r="G84" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="H84" s="5"/>
       <c r="I84" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J84" s="5"/>
       <c r="K84" s="4"/>
       <c r="L84" s="5"/>
       <c r="M84" s="4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="N84" s="5"/>
       <c r="O84" s="4"/>
@@ -5532,13 +5569,13 @@
       <c r="G85" s="4"/>
       <c r="H85" s="5"/>
       <c r="I85" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J85" s="5"/>
       <c r="K85" s="4"/>
       <c r="L85" s="5"/>
       <c r="M85" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="N85" s="5"/>
       <c r="O85" s="4"/>
@@ -5563,13 +5600,13 @@
       <c r="G86" s="4"/>
       <c r="H86" s="5"/>
       <c r="I86" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J86" s="5"/>
       <c r="K86" s="4"/>
       <c r="L86" s="5"/>
       <c r="M86" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="N86" s="5"/>
       <c r="O86" s="4"/>
@@ -5703,137 +5740,137 @@
     </row>
     <row r="91" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B91" s="1">
         <v>825</v>
       </c>
       <c r="C91" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="E91" s="2" t="s">
+      <c r="G91" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="G91" s="2" t="s">
+      <c r="I91" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="I91" s="2" t="s">
+      <c r="K91" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="K91" s="2" t="s">
+      <c r="M91" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="M91" s="2" t="s">
+      <c r="O91" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="O91" s="2" t="s">
+      <c r="Q91" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="Q91" s="2" t="s">
+      <c r="S91" s="12" t="s">
         <v>414</v>
       </c>
-      <c r="S91" s="12" t="s">
+      <c r="U91" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="U91" s="2" t="s">
+      <c r="W91" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="Y91" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="W91" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="Y91" s="2" t="s">
-        <v>417</v>
-      </c>
       <c r="AA91" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="AC91" s="2" t="s">
         <v>584</v>
-      </c>
-      <c r="AC91" s="2" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="92" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="C92" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="E92" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="E92" s="3" t="s">
+      <c r="G92" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="G92" s="3" t="s">
+      <c r="I92" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="I92" s="3" t="s">
+      <c r="K92" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="K92" s="3" t="s">
+      <c r="M92" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="M92" s="3" t="s">
+      <c r="O92" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="O92" s="3" t="s">
+      <c r="Q92" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="Q92" s="3" t="s">
+      <c r="S92" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="S92" s="3" t="s">
+      <c r="U92" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="U92" s="3" t="s">
+      <c r="W92" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="Y92" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="W92" s="3" t="s">
-        <v>555</v>
-      </c>
-      <c r="Y92" s="3" t="s">
-        <v>428</v>
-      </c>
       <c r="AA92" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="AC92" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="93" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="C93" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D93" s="5"/>
       <c r="E93" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F93" s="5"/>
       <c r="G93" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H93" s="5"/>
       <c r="I93" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J93" s="5"/>
       <c r="K93" s="4" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L93" s="5"/>
       <c r="M93" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="N93" s="5"/>
       <c r="O93" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="P93" s="5"/>
       <c r="Q93" s="6"/>
       <c r="R93" s="5"/>
       <c r="S93" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="T93" s="5"/>
       <c r="U93" s="7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="V93" s="5"/>
       <c r="W93" s="7"/>
@@ -5843,7 +5880,7 @@
     </row>
     <row r="94" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C94" s="4"/>
       <c r="D94" s="5"/>
@@ -5854,7 +5891,7 @@
       <c r="I94" s="6"/>
       <c r="J94" s="5"/>
       <c r="K94" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="L94" s="5"/>
       <c r="M94" s="7"/>
@@ -5862,15 +5899,15 @@
       <c r="O94" s="4"/>
       <c r="P94" s="5"/>
       <c r="Q94" s="4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="R94" s="5"/>
       <c r="S94" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="T94" s="5"/>
       <c r="U94" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="V94" s="5"/>
       <c r="W94" s="4"/>
@@ -5897,7 +5934,7 @@
       <c r="Q95" s="4"/>
       <c r="R95" s="5"/>
       <c r="S95" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="T95" s="5"/>
       <c r="U95" s="4"/>
@@ -6106,136 +6143,136 @@
     </row>
     <row r="103" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B103" s="1">
         <v>705</v>
       </c>
       <c r="C103" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="E103" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="E103" s="2" t="s">
+      <c r="G103" s="12" t="s">
         <v>445</v>
       </c>
-      <c r="G103" s="12" t="s">
+      <c r="I103" s="12" t="s">
         <v>446</v>
       </c>
-      <c r="I103" s="12" t="s">
+      <c r="K103" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="K103" s="12" t="s">
+      <c r="M103" s="12" t="s">
         <v>448</v>
       </c>
-      <c r="M103" s="12" t="s">
+      <c r="O103" s="12" t="s">
         <v>449</v>
       </c>
-      <c r="O103" s="12" t="s">
+      <c r="Q103" s="12" t="s">
         <v>450</v>
       </c>
-      <c r="Q103" s="12" t="s">
+      <c r="S103" s="12" t="s">
         <v>451</v>
       </c>
-      <c r="S103" s="12" t="s">
+      <c r="U103" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="U103" s="2" t="s">
-        <v>453</v>
-      </c>
       <c r="W103" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="X103" s="1">
         <v>785</v>
       </c>
       <c r="Y103" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="AA103" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="AC103" s="2" t="s">
         <v>591</v>
-      </c>
-      <c r="AC103" s="2" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="104" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="C104" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="E104" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="E104" s="3" t="s">
+      <c r="G104" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="G104" s="3" t="s">
+      <c r="I104" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="I104" s="3" t="s">
+      <c r="K104" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="K104" s="3" t="s">
+      <c r="M104" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="M104" s="3" t="s">
+      <c r="O104" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="O104" s="3" t="s">
+      <c r="Q104" s="3" t="s">
         <v>460</v>
       </c>
-      <c r="Q104" s="3" t="s">
+      <c r="S104" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="S104" s="3" t="s">
+      <c r="U104" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="U104" s="3" t="s">
-        <v>463</v>
-      </c>
       <c r="W104" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="Y104" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="AA104" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="AC104" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="105" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="C105" s="4" t="s">
         <v>464</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>465</v>
       </c>
       <c r="D105" s="5"/>
       <c r="E105" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F105" s="5"/>
       <c r="G105" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="H105" s="5"/>
       <c r="I105" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="J105" s="5"/>
       <c r="K105" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="L105" s="5"/>
       <c r="M105" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="N105" s="5"/>
       <c r="O105" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="P105" s="5"/>
       <c r="Q105" s="6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="R105" s="5"/>
       <c r="S105" s="4"/>
@@ -6249,34 +6286,34 @@
     </row>
     <row r="106" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="C106" s="4" t="s">
         <v>473</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>474</v>
       </c>
       <c r="D106" s="5"/>
       <c r="E106" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F106" s="5"/>
       <c r="G106" s="4" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="H106" s="5"/>
       <c r="I106" s="6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J106" s="5"/>
       <c r="K106" s="6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="L106" s="5"/>
       <c r="M106" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="N106" s="5"/>
       <c r="O106" s="4" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="P106" s="5"/>
       <c r="Q106" s="4"/>
@@ -6293,29 +6330,29 @@
     <row r="107" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="C107" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D107" s="5"/>
       <c r="E107" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F107" s="5"/>
       <c r="G107" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H107" s="5"/>
       <c r="I107" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="J107" s="5"/>
       <c r="K107" s="7"/>
       <c r="L107" s="5"/>
       <c r="M107" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="N107" s="5"/>
       <c r="O107" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="P107" s="5"/>
       <c r="Q107" s="4"/>
@@ -6332,17 +6369,17 @@
     <row r="108" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="C108" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D108" s="5"/>
       <c r="E108" s="4"/>
       <c r="F108" s="5"/>
       <c r="G108" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H108" s="5"/>
       <c r="I108" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="J108" s="5"/>
       <c r="K108" s="4"/>
@@ -6350,7 +6387,7 @@
       <c r="M108" s="4"/>
       <c r="N108" s="5"/>
       <c r="O108" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="P108" s="5"/>
       <c r="Q108" s="4"/>
@@ -6492,7 +6529,7 @@
     <row r="114" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="115" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="Y115" s="1">
         <v>988</v>
@@ -6506,38 +6543,38 @@
     </row>
     <row r="116" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="X116" s="1">
         <v>655</v>
       </c>
       <c r="Y116" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="AA116" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="AA116" s="2" t="s">
+      <c r="AC116" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="AC116" s="2" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="117" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Y117" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="AA117" s="3" t="s">
         <v>597</v>
       </c>
-      <c r="AA117" s="3" t="s">
-        <v>598</v>
-      </c>
       <c r="AC117" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="118" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="Y118" s="4"/>
       <c r="AA118" s="4"/>
@@ -6545,7 +6582,7 @@
     </row>
     <row r="119" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Y119" s="4"/>
       <c r="AA119" s="4"/>
@@ -6553,7 +6590,7 @@
     </row>
     <row r="120" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Y120" s="4"/>
       <c r="AA120" s="4"/>
@@ -6561,7 +6598,7 @@
     </row>
     <row r="121" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Y121" s="4"/>
       <c r="AA121" s="4"/>
@@ -6569,7 +6606,7 @@
     </row>
     <row r="122" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Y122" s="4"/>
       <c r="AA122" s="4"/>
@@ -6577,7 +6614,7 @@
     </row>
     <row r="123" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="Y123" s="4"/>
       <c r="AA123" s="4"/>
@@ -6585,7 +6622,7 @@
     </row>
     <row r="124" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Y124" s="4"/>
       <c r="AA124" s="4"/>
@@ -6593,7 +6630,7 @@
     </row>
     <row r="125" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Y125" s="4"/>
       <c r="AA125" s="4"/>
@@ -6601,7 +6638,7 @@
     </row>
     <row r="126" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="Y126" s="8"/>
       <c r="AA126" s="8"/>
@@ -6609,118 +6646,118 @@
     </row>
     <row r="127" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A127" s="9" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="128" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A128" s="9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="9" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="8" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="9" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="10" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>